<commit_message>
updated _images, updated_ notebook
</commit_message>
<xml_diff>
--- a/Capstone_results.xlsx
+++ b/Capstone_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a08b256d5a00faca/Documents/School/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a08b256d5a00faca/Documents/School/Final_Capstone_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{A1FDE708-B617-4BD6-B7E9-1CFC88CCCA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{075D1E4F-7C1C-486D-B99B-41696D633C4F}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{A1FDE708-B617-4BD6-B7E9-1CFC88CCCA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{615D844D-C794-47CE-82D1-0980C1D48895}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74C1B205-F606-4DDE-A949-DBF75447989C}"/>
   </bookViews>
@@ -132,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,18 +153,29 @@
       <name val="Var(--jp-code-font-family)"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Century Gothic"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Century Gothic"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -181,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -204,45 +215,45 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8124,6 +8135,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Ion">
   <a:themeElements>
@@ -8419,8 +8434,8 @@
   </sheetPr>
   <dimension ref="A2:O32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -8437,73 +8452,73 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="14">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:15" ht="14">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="7">
         <v>348993.43222832202</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="8">
         <v>0.15670000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:15" ht="14">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="7">
         <v>353875.39088398399</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="8">
         <v>0.16844999999999999</v>
       </c>
       <c r="J4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:15" ht="14">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="7">
         <v>223798.139329094</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="9">
         <v>0.65322111740105404</v>
       </c>
       <c r="K5" t="s">
@@ -8522,127 +8537,127 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:15" ht="14">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="7">
         <v>228260.934411725</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="9">
         <v>0.65402393244023105</v>
       </c>
       <c r="J6" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="2">
         <v>0.88</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="2">
         <v>0.95400664487275499</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="2">
         <v>0.96</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="2">
         <v>0.91</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="2">
         <v>0.93</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:15" ht="14">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="7">
         <v>325847.39363578899</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="9">
         <v>0.26486313309530701</v>
       </c>
       <c r="J7" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="2">
         <v>0.88</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="2">
         <v>0.95565055504755503</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="2">
         <v>0.96</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="2">
         <v>0.91</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="2">
         <v>0.93</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:15" ht="14">
+      <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="7">
         <v>329217.60477420501</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="9">
         <v>0.28030418332375401</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:15" ht="14">
+      <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="7">
         <v>264288.28467960801</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="9">
         <v>0.51638971951525403</v>
       </c>
       <c r="J9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:15" ht="14">
+      <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="7">
         <v>267398.79916780803</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="9">
         <v>0.52520976116616402</v>
       </c>
       <c r="K10" t="s">
@@ -8661,158 +8676,158 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:15" ht="14">
+      <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="7">
         <v>369642.31900703802</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="9">
         <v>5.3974000237213798E-2</v>
       </c>
       <c r="J11" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>133737.51132267099</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <v>81503.769650442497</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="1">
         <v>78111.956680200994</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="1">
         <v>113947.968105104</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="1">
         <v>101433.450851366</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:15" ht="14">
+      <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="7">
         <v>377287.89305751101</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="9">
         <v>5.4789331347668099E-2</v>
       </c>
       <c r="J12" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <v>133737.10177390301</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <v>81724.572253321006</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="1">
         <v>80014.384506464805</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="1">
         <v>114102.600948537</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="1">
         <v>102996.31462004699</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:15" ht="14">
+      <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="7">
         <v>133737.51132267099</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="9">
         <v>0.87616421128093702</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:15" ht="14">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="7">
         <v>133737.10177390301</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="9">
         <v>0.88123548727690704</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:15" ht="14">
+      <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="11">
         <v>207191.89167234101</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="9">
         <v>0.70277508531275101</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:15" ht="14">
+      <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="11">
         <v>209507.29026932101</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="9">
         <v>0.70853852651376004</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:15" ht="14">
+      <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="7">
         <v>81503.769650442497</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="9">
         <v>0.95400664487275499</v>
       </c>
       <c r="J17" t="s">
@@ -8822,37 +8837,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:15" ht="14">
+      <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="7">
         <v>81724.572253321006</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="9">
         <v>0.95565055504755503</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:15" ht="14">
+      <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="7">
         <v>78111.956680200994</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="9">
         <v>0.95775505648870796</v>
       </c>
       <c r="K19" t="s">
@@ -8871,141 +8886,141 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:15" ht="14">
+      <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="7">
         <v>80014.384506464805</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="9">
         <v>0.95748726806728801</v>
       </c>
       <c r="J20" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="2">
         <v>0.7</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="2">
         <v>0.76</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="2">
         <v>0.77</v>
       </c>
-      <c r="N20" s="4">
+      <c r="N20" s="2">
         <v>0.74</v>
       </c>
-      <c r="O20" s="4">
+      <c r="O20" s="2">
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:15" ht="14">
+      <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="11">
         <v>186117.02325801799</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="9">
         <v>0.76016536775413401</v>
       </c>
       <c r="J21" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="2">
         <v>0.71</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="2">
         <v>0.77</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="2">
         <v>0.77</v>
       </c>
-      <c r="N21" s="4">
+      <c r="N21" s="2">
         <v>0.74</v>
       </c>
-      <c r="O21" s="8">
+      <c r="O21" s="4">
         <v>0.76</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:15" ht="14">
+      <c r="A22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="11">
         <v>187424.369632599</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="9">
         <v>0.76674283428640999</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:15" ht="14">
+      <c r="A23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="11">
         <v>180862.43346987001</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="9">
         <v>0.77351656680677305</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:15" ht="14">
+      <c r="A24" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="11">
         <v>187954.32914785101</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="9">
         <v>0.76542185747124103</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:15" ht="14">
+      <c r="A25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="7">
         <v>113947.968105104</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="9">
         <v>0.91010141197154404</v>
       </c>
       <c r="J25" t="s">
@@ -9015,37 +9030,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:15" ht="14">
+      <c r="A26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="7">
         <v>114102.600948537</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="9">
         <v>0.91354821495829097</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:15" ht="14">
+      <c r="A27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="7">
         <v>101433.450851366</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="9">
         <v>0.928763577413389</v>
       </c>
       <c r="K27" t="s">
@@ -9064,130 +9079,130 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:15" ht="14">
+      <c r="A28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="7">
         <v>102996.31462004699</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="9">
         <v>0.929558880907563</v>
       </c>
       <c r="J28" t="s">
         <v>6</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="1">
         <v>207191.89167234101</v>
       </c>
-      <c r="L28" s="6">
+      <c r="L28" s="3">
         <v>186117.02325801799</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M28" s="3">
         <v>180862.43346987001</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N28" s="3">
         <v>194734.277003567</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O28" s="3">
         <v>189585.94499140399</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:15" ht="14">
+      <c r="A29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="11">
         <v>194734.277003567</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="9">
         <v>0.73744245379178996</v>
       </c>
       <c r="J29" t="s">
         <v>7</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="1">
         <v>209507.29026932101</v>
       </c>
-      <c r="L29" s="6">
+      <c r="L29" s="3">
         <v>187424.369632599</v>
       </c>
-      <c r="M29" s="6">
+      <c r="M29" s="3">
         <v>187954.32914785101</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29" s="3">
         <v>195971.846440933</v>
       </c>
-      <c r="O29" s="9">
+      <c r="O29" s="5">
         <v>191117.49907541601</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:15" ht="14">
+      <c r="A30" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="11">
         <v>195971.846440933</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="9">
         <v>0.74498234631927296</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:15" ht="14">
+      <c r="A31" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="11">
         <v>189585.94499140399</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="9">
         <v>0.75114178869971404</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:15" ht="14">
+      <c r="A32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="12">
         <v>191117.49907541601</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="9">
         <v>0.75745977064022296</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:E32" xr:uid="{8894E937-28F0-4274-879B-2ECBDAF7CC6B}"/>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update_readme, add_excel_file and images
</commit_message>
<xml_diff>
--- a/Capstone_results.xlsx
+++ b/Capstone_results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a08b256d5a00faca/Documents/School/Final_Capstone_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{A1FDE708-B617-4BD6-B7E9-1CFC88CCCA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{615D844D-C794-47CE-82D1-0980C1D48895}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="13_ncr:1_{A1FDE708-B617-4BD6-B7E9-1CFC88CCCA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C28348CA-6E9E-451C-9787-83BF10B8609F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74C1B205-F606-4DDE-A949-DBF75447989C}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
-    <sheet name="Charts" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="conclusion" sheetId="4" r:id="rId2"/>
+    <sheet name="Charts" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$2:$E$32</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="27">
   <si>
     <t>Model</t>
   </si>
@@ -124,6 +125,12 @@
   <si>
     <t>Elastic Net-degree 8</t>
   </si>
+  <si>
+    <t>Model (Indpendent Variables)</t>
+  </si>
+  <si>
+    <t>Model (No Attendance)</t>
+  </si>
 </sst>
 </file>
 
@@ -178,7 +185,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +198,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -215,12 +234,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -255,6 +296,38 @@
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8435,7 +8508,7 @@
   <dimension ref="A2:O32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G24" sqref="G23:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9209,6 +9282,300 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6854CE8E-0AC3-4DC0-B34F-CA23BA9272A8}">
+  <dimension ref="B3:G20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.58203125" customWidth="1"/>
+    <col min="4" max="4" width="8.58203125" customWidth="1"/>
+    <col min="5" max="5" width="1.6640625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.58203125" customWidth="1"/>
+    <col min="7" max="7" width="8.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" ht="14">
+      <c r="C3" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="2:7" ht="14">
+      <c r="B4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="14">
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7">
+        <v>133737.51132267099</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.87616421128093702</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="7">
+        <v>133737.10177390301</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.88123548727690704</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="14">
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7">
+        <v>81503.769650442497</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.95400664487275499</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="7">
+        <v>81724.572253321006</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.95565055504755503</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="14">
+      <c r="B7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="14">
+        <v>78111.956680200994</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0.95775505648870796</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="14">
+        <v>80014.384506464805</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0.95748726806728801</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="14">
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="7">
+        <v>113947.968105104</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.91010141197154404</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="7">
+        <v>114102.600948537</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0.91354821495829097</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="14">
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7">
+        <v>101433.450851366</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.928763577413389</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="7">
+        <v>102996.31462004699</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0.929558880907563</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="14">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="2:7" ht="14">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="2:7" ht="14">
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="2:7" ht="14">
+      <c r="C13" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="2:7" ht="14">
+      <c r="B14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="14">
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="11">
+        <v>207191.89167234101</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.70277508531275101</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="11">
+        <v>209507.29026932101</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.70853852651376004</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="14">
+      <c r="B16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="14">
+        <v>186117.02325801799</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0.76016536775413401</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="14">
+        <v>187424.369632599</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0.76674283428640999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="14">
+      <c r="B17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="11">
+        <v>180862.43346987001</v>
+      </c>
+      <c r="D17" s="17">
+        <v>0.77351656680677305</v>
+      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="11">
+        <v>187954.32914785101</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0.76542185747124103</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="14">
+      <c r="B18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="11">
+        <v>194734.277003567</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.73744245379178996</v>
+      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="11">
+        <v>195971.846440933</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0.74498234631927296</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="14">
+      <c r="B19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="11">
+        <v>189585.94499140399</v>
+      </c>
+      <c r="D19" s="23">
+        <v>0.75114178869971404</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="12">
+        <v>191117.49907541601</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0.75745977064022296</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="E20" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D33905-2B3B-437E-8172-63E9242451CD}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9223,7 +9590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6635124-B345-437F-B451-35B5EF41BF3D}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>